<commit_message>
Prevent resizing, center window
</commit_message>
<xml_diff>
--- a/flappy/res/leaderboard.xlsx
+++ b/flappy/res/leaderboard.xlsx
@@ -1268,21 +1268,21 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Abhijit</t>
+          <t>Hello</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Not Applicable</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>Not Applicable</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="E34" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="35">
@@ -1293,7 +1293,7 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>mB</t>
+          <t>Abhijit</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
@@ -1307,7 +1307,7 @@
         </is>
       </c>
       <c r="E35" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="36">
@@ -1318,7 +1318,7 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Mama</t>
+          <t>mB</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
@@ -1343,7 +1343,7 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>t</t>
+          <t>Mama</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
@@ -1357,7 +1357,7 @@
         </is>
       </c>
       <c r="E37" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="38">
@@ -1368,7 +1368,7 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>t</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
@@ -1382,7 +1382,7 @@
         </is>
       </c>
       <c r="E38" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="39">
@@ -1393,7 +1393,7 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>AB</t>
+          <t>B</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
@@ -1418,7 +1418,7 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>Ab</t>
+          <t>AB</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
@@ -1443,17 +1443,17 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Abhijit</t>
+          <t>Ab</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>Not Applicable</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>Not Applicable</t>
         </is>
       </c>
       <c r="E41" t="n">

</xml_diff>

<commit_message>
Fix cx_freeze on mac
</commit_message>
<xml_diff>
--- a/flappy/res/leaderboard.xlsx
+++ b/flappy/res/leaderboard.xlsx
@@ -713,22 +713,22 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Teacher</t>
+          <t>Student</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Abhi</t>
+          <t>Aditya</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Not Applicable</t>
+          <t>7</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Not Applicable</t>
+          <t>E</t>
         </is>
       </c>
       <c r="E12" t="n">
@@ -743,7 +743,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>hy</t>
+          <t>Abhi</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -763,22 +763,22 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Student</t>
+          <t>Teacher</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Aditya</t>
+          <t>hy</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>Not Applicable</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>Not Applicable</t>
         </is>
       </c>
       <c r="E14" t="n">
@@ -993,7 +993,7 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>buck</t>
+          <t>Abhijit</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
@@ -1018,7 +1018,7 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>f</t>
+          <t>buck</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
@@ -1043,7 +1043,7 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Abhijit</t>
+          <t>f</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
@@ -1268,7 +1268,7 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>AA</t>
+          <t>nk</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
@@ -1293,7 +1293,7 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>nk</t>
+          <t>AA</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
@@ -1318,21 +1318,21 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>AAAA</t>
+          <t>mB</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>Not Applicable</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>Not Applicable</t>
         </is>
       </c>
       <c r="E36" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="37">
@@ -1343,7 +1343,7 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>mB</t>
+          <t>Mama</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
@@ -1368,17 +1368,17 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Mama</t>
+          <t>A</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>Not Applicable</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>Not Applicable</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="E38" t="n">

</xml_diff>

<commit_message>
Make code python3.8 compatible
</commit_message>
<xml_diff>
--- a/flappy/res/leaderboard.xlsx
+++ b/flappy/res/leaderboard.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E44"/>
+  <dimension ref="A1:E46"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -643,37 +643,37 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>boo</t>
+          <t>AAA</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Not Applicable</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Not Applicable</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="E9" t="n">
-        <v>42</v>
+        <v>45</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Student</t>
+          <t>Teacher</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Madhu</t>
+          <t>boo</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>Not Applicable</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -682,23 +682,23 @@
         </is>
       </c>
       <c r="E10" t="n">
-        <v>38</v>
+        <v>42</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Teacher</t>
+          <t>Student</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>rl</t>
+          <t>Madhu</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Not Applicable</t>
+          <t>5</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -707,32 +707,32 @@
         </is>
       </c>
       <c r="E11" t="n">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Student</t>
+          <t>Teacher</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Aditya</t>
+          <t>rl</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>Not Applicable</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>Not Applicable</t>
         </is>
       </c>
       <c r="E12" t="n">
-        <v>29</v>
+        <v>37</v>
       </c>
     </row>
     <row r="13">
@@ -743,7 +743,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Abhi</t>
+          <t>hy</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -768,7 +768,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>hy</t>
+          <t>Abhi</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -793,7 +793,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>Aditya</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -803,32 +803,32 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>e</t>
+          <t>E</t>
         </is>
       </c>
       <c r="E15" t="n">
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Teacher</t>
+          <t>Student</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>3</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Not Applicable</t>
+          <t>7</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>Not Applicable</t>
+          <t>e</t>
         </is>
       </c>
       <c r="E16" t="n">
@@ -843,7 +843,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>r</t>
+          <t>M</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
@@ -857,7 +857,7 @@
         </is>
       </c>
       <c r="E17" t="n">
-        <v>24</v>
+        <v>27</v>
       </c>
     </row>
     <row r="18">
@@ -868,21 +868,21 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>r</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>Not Applicable</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>Not Applicable</t>
         </is>
       </c>
       <c r="E18" t="n">
-        <v>20</v>
+        <v>24</v>
       </c>
     </row>
     <row r="19">
@@ -893,7 +893,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>drt</t>
+          <t>AAA</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
@@ -907,32 +907,32 @@
         </is>
       </c>
       <c r="E19" t="n">
-        <v>17</v>
+        <v>22</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Student</t>
+          <t>Teacher</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Aditya</t>
+          <t>A</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>Not Applicable</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>Not Applicable</t>
         </is>
       </c>
       <c r="E20" t="n">
-        <v>15</v>
+        <v>20</v>
       </c>
     </row>
     <row r="21">
@@ -943,7 +943,7 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>AAA</t>
+          <t>Ab</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
@@ -957,7 +957,7 @@
         </is>
       </c>
       <c r="E21" t="n">
-        <v>15</v>
+        <v>19</v>
       </c>
     </row>
     <row r="22">
@@ -968,7 +968,7 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>drt</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
@@ -982,32 +982,32 @@
         </is>
       </c>
       <c r="E22" t="n">
-        <v>13</v>
+        <v>17</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Teacher</t>
+          <t>Student</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>rbb</t>
+          <t>Aditya</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Not Applicable</t>
+          <t>6</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>Not Applicable</t>
+          <t>B</t>
         </is>
       </c>
       <c r="E23" t="n">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="24">
@@ -1018,7 +1018,7 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>buck</t>
+          <t>rbb</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
@@ -1032,7 +1032,7 @@
         </is>
       </c>
       <c r="E24" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="25">
@@ -1068,7 +1068,7 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>MB</t>
+          <t>buck</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
@@ -1082,7 +1082,7 @@
         </is>
       </c>
       <c r="E26" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="27">
@@ -1093,7 +1093,7 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>d</t>
+          <t>MB</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
@@ -1107,7 +1107,7 @@
         </is>
       </c>
       <c r="E27" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="28">
@@ -1118,7 +1118,7 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>im</t>
+          <t>d</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
@@ -1132,7 +1132,7 @@
         </is>
       </c>
       <c r="E28" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="29">
@@ -1143,7 +1143,7 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Abhijit</t>
+          <t>im</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
@@ -1157,7 +1157,7 @@
         </is>
       </c>
       <c r="E29" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="30">
@@ -1168,7 +1168,7 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Abh</t>
+          <t>Abhijit</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
@@ -1182,7 +1182,7 @@
         </is>
       </c>
       <c r="E30" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="31">
@@ -1238,12 +1238,12 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Parent</t>
+          <t>Teacher</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Aditya</t>
+          <t>Abh</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
@@ -1257,18 +1257,18 @@
         </is>
       </c>
       <c r="E33" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Teacher</t>
+          <t>Parent</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>AAAA</t>
+          <t>Aditya</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
@@ -1282,7 +1282,7 @@
         </is>
       </c>
       <c r="E34" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="35">
@@ -1293,7 +1293,7 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>AA</t>
+          <t>AAAA</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
@@ -1307,7 +1307,7 @@
         </is>
       </c>
       <c r="E35" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="36">
@@ -1318,7 +1318,7 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>nk</t>
+          <t>AAAAA</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
@@ -1332,7 +1332,7 @@
         </is>
       </c>
       <c r="E36" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="37">
@@ -1343,7 +1343,7 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>mB</t>
+          <t>AA</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
@@ -1357,7 +1357,7 @@
         </is>
       </c>
       <c r="E37" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="38">
@@ -1368,7 +1368,7 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Mama</t>
+          <t>nk</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
@@ -1382,7 +1382,7 @@
         </is>
       </c>
       <c r="E38" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="39">
@@ -1393,7 +1393,7 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>t</t>
+          <t>Montu</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
@@ -1407,32 +1407,32 @@
         </is>
       </c>
       <c r="E39" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Student</t>
+          <t>Teacher</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>AAAAA</t>
+          <t>mB</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>LKG</t>
+          <t>Not Applicable</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>Not Applicable</t>
         </is>
       </c>
       <c r="E40" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="41">
@@ -1443,7 +1443,7 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>Mama</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
@@ -1457,7 +1457,7 @@
         </is>
       </c>
       <c r="E41" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="42">
@@ -1468,7 +1468,7 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>AB</t>
+          <t>t</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
@@ -1482,32 +1482,32 @@
         </is>
       </c>
       <c r="E42" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>Teacher</t>
+          <t>Student</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Ab</t>
+          <t>AAAAA</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Not Applicable</t>
+          <t>LKG</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>Not Applicable</t>
+          <t>E</t>
         </is>
       </c>
       <c r="E43" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="44">
@@ -1518,20 +1518,70 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>Not Applicable</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>Not Applicable</t>
+        </is>
+      </c>
+      <c r="E44" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>Teacher</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>AB</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>Not Applicable</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>Not Applicable</t>
+        </is>
+      </c>
+      <c r="E45" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>Teacher</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
           <t>Ad</t>
         </is>
       </c>
-      <c r="C44" t="inlineStr">
-        <is>
-          <t>Not Applicable</t>
-        </is>
-      </c>
-      <c r="D44" t="inlineStr">
-        <is>
-          <t>Not Applicable</t>
-        </is>
-      </c>
-      <c r="E44" t="n">
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>Not Applicable</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>Not Applicable</t>
+        </is>
+      </c>
+      <c r="E46" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>